<commit_message>
Updates for 2024 survey
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024_99_z_state_survey.xlsx
+++ b/statistics_files/2024/2024_99_z_state_survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D41B91-ACFF-400D-B165-736FE923A833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792F9FD1-63AE-4933-A18A-A08628DBCDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="717" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="717" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="State Survey-2024 data" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'State Survey-2021 data'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'State Survey-2022 data'!$A$1:$M$55</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'State Survey-2023 data'!$A$1:$N$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'State Survey-2024 data'!$A$1:$N$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'State Survey-2024 data'!$A$1:$V$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="191">
   <si>
     <t>branchcode</t>
   </si>
@@ -579,6 +579,51 @@
   <si>
     <t>Question 9.4 - total of all other materials at end of 2024</t>
   </si>
+  <si>
+    <t>Question 11.3 - does your library offer automatic renewal?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Question 11.4b - circulation "Other physical items"</t>
+  </si>
+  <si>
+    <t>Question 11.13 - borrowing requests that go unfilled</t>
+  </si>
+  <si>
+    <t>undeterminable in Koha</t>
+  </si>
+  <si>
+    <t>Question 11.17 - borrowing requests that go unfilled</t>
+  </si>
+  <si>
+    <t>Question 11.1 - circulation of adult print materials</t>
+  </si>
+  <si>
+    <t>Question 11.1a - circulation of adult non-print materials</t>
+  </si>
+  <si>
+    <t>Question 2.3 - Number of registered users</t>
+  </si>
+  <si>
+    <t>Question 11.2 - total circulation of non-adult print materials</t>
+  </si>
+  <si>
+    <t>Question 11.2a - total circulation of non-adult non-print materials</t>
+  </si>
+  <si>
+    <t>Question 11.2b - total circulation of non-adult materials</t>
+  </si>
+  <si>
+    <t>Question 11.4a - total circulation of print materials</t>
+  </si>
+  <si>
+    <t>Question 11.4c - total physical item circulation</t>
+  </si>
+  <si>
+    <t>Question 11.1b - total circulation of adult materials</t>
+  </si>
 </sst>
 </file>
 
@@ -727,7 +772,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -955,6 +1000,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1138,7 +1189,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1196,6 +1247,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1530,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72339743-29E1-4007-A046-5505500D715D}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:W58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -1542,15 +1617,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" style="7" customWidth="1"/>
-    <col min="2" max="14" width="16.7109375" style="7" customWidth="1"/>
+    <col min="2" max="20" width="16.7109375" style="7" customWidth="1"/>
+    <col min="21" max="21" width="23.85546875" style="7" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" style="7" customWidth="1"/>
+    <col min="23" max="23" width="23.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>56</v>
+        <v>184</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>170</v>
@@ -1573,23 +1651,50 @@
       <c r="I1" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="J1" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>61</v>
+      <c r="J1" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>183</v>
       </c>
       <c r="L1" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="M1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="T1" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="U1" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="V1" s="25" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W1" s="26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>106</v>
       </c>
@@ -1618,22 +1723,51 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
+        <v>20742</v>
+      </c>
+      <c r="K2" s="1">
+        <v>10148</v>
+      </c>
+      <c r="L2" s="1">
         <v>30890</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="1">
+        <v>35362</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2991</v>
+      </c>
+      <c r="O2" s="1">
         <v>38353</v>
       </c>
-      <c r="L2" s="14">
+      <c r="P2" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="14">
+        <f>SUM(J2,M2)</f>
+        <v>56104</v>
+      </c>
+      <c r="R2" s="14">
         <v>673</v>
       </c>
-      <c r="M2" s="1">
+      <c r="S2" s="14">
+        <f>SUM(L2,O2,R2)</f>
+        <v>69916</v>
+      </c>
+      <c r="T2" s="1">
         <v>10922</v>
       </c>
-      <c r="N2" s="1">
+      <c r="U2" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V2" s="1">
         <v>11835</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W2" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
         <v>107</v>
       </c>
@@ -1662,22 +1796,51 @@
         <v>0</v>
       </c>
       <c r="J3" s="2">
+        <v>12777</v>
+      </c>
+      <c r="K3" s="2">
+        <v>3250</v>
+      </c>
+      <c r="L3" s="2">
         <v>16027</v>
       </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2">
+        <v>22842</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1385</v>
+      </c>
+      <c r="O3" s="2">
         <v>24227</v>
       </c>
-      <c r="L3" s="15">
+      <c r="P3" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q3" s="15">
+        <f t="shared" ref="Q3:Q55" si="0">SUM(J3,M3)</f>
+        <v>35619</v>
+      </c>
+      <c r="R3" s="15">
         <v>1295</v>
       </c>
-      <c r="M3" s="2">
+      <c r="S3" s="15">
+        <f t="shared" ref="S3:S55" si="1">SUM(L3,O3,R3)</f>
+        <v>41549</v>
+      </c>
+      <c r="T3" s="2">
         <v>3882</v>
       </c>
-      <c r="N3" s="2">
+      <c r="U3" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V3" s="2">
         <v>5218</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W3" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>108</v>
       </c>
@@ -1706,22 +1869,51 @@
         <v>36</v>
       </c>
       <c r="J4" s="1">
+        <v>28529</v>
+      </c>
+      <c r="K4" s="1">
+        <v>12304</v>
+      </c>
+      <c r="L4" s="1">
         <v>40833</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
+        <v>61973</v>
+      </c>
+      <c r="N4" s="1">
+        <v>5108</v>
+      </c>
+      <c r="O4" s="1">
         <v>67081</v>
       </c>
-      <c r="L4" s="14">
+      <c r="P4" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q4" s="14">
+        <f t="shared" si="0"/>
+        <v>90502</v>
+      </c>
+      <c r="R4" s="14">
         <v>2435</v>
       </c>
-      <c r="M4" s="1">
+      <c r="S4" s="14">
+        <f t="shared" si="1"/>
+        <v>110349</v>
+      </c>
+      <c r="T4" s="1">
         <v>10614</v>
       </c>
-      <c r="N4" s="1">
+      <c r="U4" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V4" s="1">
         <v>9894</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W4" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>109</v>
       </c>
@@ -1750,22 +1942,51 @@
         <v>0</v>
       </c>
       <c r="J5" s="2">
+        <v>607</v>
+      </c>
+      <c r="K5" s="2">
+        <v>342</v>
+      </c>
+      <c r="L5" s="2">
         <v>949</v>
       </c>
-      <c r="K5" s="2">
+      <c r="M5" s="2">
+        <v>965</v>
+      </c>
+      <c r="N5" s="2">
+        <v>100</v>
+      </c>
+      <c r="O5" s="2">
         <v>1065</v>
       </c>
-      <c r="L5" s="15">
+      <c r="P5" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q5" s="15">
+        <f t="shared" si="0"/>
+        <v>1572</v>
+      </c>
+      <c r="R5" s="15">
         <v>2</v>
       </c>
-      <c r="M5" s="2">
+      <c r="S5" s="15">
+        <f t="shared" si="1"/>
+        <v>2016</v>
+      </c>
+      <c r="T5" s="2">
         <v>1094</v>
       </c>
-      <c r="N5" s="2">
+      <c r="U5" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V5" s="2">
         <v>303</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W5" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>110</v>
       </c>
@@ -1794,22 +2015,51 @@
         <v>59</v>
       </c>
       <c r="J6" s="1">
+        <v>22640</v>
+      </c>
+      <c r="K6" s="1">
+        <v>7870</v>
+      </c>
+      <c r="L6" s="1">
         <v>30510</v>
       </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
+        <v>37910</v>
+      </c>
+      <c r="N6" s="1">
+        <v>3386</v>
+      </c>
+      <c r="O6" s="1">
         <v>41296</v>
       </c>
-      <c r="L6" s="14">
+      <c r="P6" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" si="0"/>
+        <v>60550</v>
+      </c>
+      <c r="R6" s="14">
         <v>1502</v>
       </c>
-      <c r="M6" s="1">
+      <c r="S6" s="14">
+        <f t="shared" si="1"/>
+        <v>73308</v>
+      </c>
+      <c r="T6" s="1">
         <v>12756</v>
       </c>
-      <c r="N6" s="1">
+      <c r="U6" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V6" s="1">
         <v>9124</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W6" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>111</v>
       </c>
@@ -1838,22 +2088,51 @@
         <v>0</v>
       </c>
       <c r="J7" s="2">
+        <v>2625</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1492</v>
+      </c>
+      <c r="L7" s="2">
         <v>4117</v>
       </c>
-      <c r="K7" s="2">
+      <c r="M7" s="2">
+        <v>3623</v>
+      </c>
+      <c r="N7" s="2">
+        <v>625</v>
+      </c>
+      <c r="O7" s="2">
         <v>4248</v>
       </c>
-      <c r="L7" s="15">
+      <c r="P7" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q7" s="15">
+        <f t="shared" si="0"/>
+        <v>6248</v>
+      </c>
+      <c r="R7" s="15">
         <v>127</v>
       </c>
-      <c r="M7" s="2">
+      <c r="S7" s="15">
+        <f t="shared" si="1"/>
+        <v>8492</v>
+      </c>
+      <c r="T7" s="2">
         <v>1699</v>
       </c>
-      <c r="N7" s="2">
+      <c r="U7" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V7" s="2">
         <v>1817</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W7" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>112</v>
       </c>
@@ -1882,22 +2161,51 @@
         <v>0</v>
       </c>
       <c r="J8" s="1">
+        <v>3978</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1242</v>
+      </c>
+      <c r="L8" s="1">
         <v>5220</v>
       </c>
-      <c r="K8" s="1">
+      <c r="M8" s="1">
+        <v>3089</v>
+      </c>
+      <c r="N8" s="1">
+        <v>492</v>
+      </c>
+      <c r="O8" s="1">
         <v>3581</v>
       </c>
-      <c r="L8" s="14">
+      <c r="P8" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q8" s="14">
+        <f t="shared" si="0"/>
+        <v>7067</v>
+      </c>
+      <c r="R8" s="14">
         <v>26</v>
       </c>
-      <c r="M8" s="1">
+      <c r="S8" s="14">
+        <f t="shared" si="1"/>
+        <v>8827</v>
+      </c>
+      <c r="T8" s="1">
         <v>1878</v>
       </c>
-      <c r="N8" s="1">
+      <c r="U8" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V8" s="1">
         <v>1260</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W8" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>113</v>
       </c>
@@ -1926,22 +2234,51 @@
         <v>0</v>
       </c>
       <c r="J9" s="2">
+        <v>2272</v>
+      </c>
+      <c r="K9" s="2">
+        <v>229</v>
+      </c>
+      <c r="L9" s="2">
         <v>2501</v>
       </c>
-      <c r="K9" s="2">
+      <c r="M9" s="2">
+        <v>1571</v>
+      </c>
+      <c r="N9" s="2">
+        <v>82</v>
+      </c>
+      <c r="O9" s="2">
         <v>1653</v>
       </c>
-      <c r="L9" s="15">
-        <v>0</v>
-      </c>
-      <c r="M9" s="2">
+      <c r="P9" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q9" s="15">
+        <f t="shared" si="0"/>
+        <v>3843</v>
+      </c>
+      <c r="R9" s="15">
+        <v>0</v>
+      </c>
+      <c r="S9" s="15">
+        <f t="shared" si="1"/>
+        <v>4154</v>
+      </c>
+      <c r="T9" s="2">
         <v>647</v>
       </c>
-      <c r="N9" s="2">
+      <c r="U9" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V9" s="2">
         <v>340</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W9" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>114</v>
       </c>
@@ -1970,22 +2307,51 @@
         <v>0</v>
       </c>
       <c r="J10" s="1">
+        <v>139</v>
+      </c>
+      <c r="K10" s="1">
+        <v>9</v>
+      </c>
+      <c r="L10" s="1">
         <v>148</v>
       </c>
-      <c r="K10" s="1">
+      <c r="M10" s="1">
+        <v>1374</v>
+      </c>
+      <c r="N10" s="1">
+        <v>26</v>
+      </c>
+      <c r="O10" s="1">
         <v>1400</v>
       </c>
-      <c r="L10" s="14">
+      <c r="P10" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" si="0"/>
+        <v>1513</v>
+      </c>
+      <c r="R10" s="14">
         <v>3</v>
       </c>
-      <c r="M10" s="1">
+      <c r="S10" s="14">
+        <f t="shared" si="1"/>
+        <v>1551</v>
+      </c>
+      <c r="T10" s="1">
         <v>475</v>
       </c>
-      <c r="N10" s="1">
+      <c r="U10" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W10" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>115</v>
       </c>
@@ -2019,7 +2385,7 @@
       <c r="K11" s="2">
         <v>0</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="2">
         <v>0</v>
       </c>
       <c r="M11" s="2">
@@ -2028,8 +2394,37 @@
       <c r="N11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+      <c r="P11" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R11" s="15">
+        <v>0</v>
+      </c>
+      <c r="S11" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
+      <c r="W11" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>116</v>
       </c>
@@ -2058,22 +2453,51 @@
         <v>42</v>
       </c>
       <c r="J12" s="3">
+        <v>405</v>
+      </c>
+      <c r="K12" s="3">
+        <v>240</v>
+      </c>
+      <c r="L12" s="3">
         <v>645</v>
       </c>
-      <c r="K12" s="3">
+      <c r="M12" s="3">
+        <v>481</v>
+      </c>
+      <c r="N12" s="3">
+        <v>77</v>
+      </c>
+      <c r="O12" s="3">
         <v>558</v>
       </c>
-      <c r="L12" s="16">
+      <c r="P12" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q12" s="16">
+        <f t="shared" si="0"/>
+        <v>886</v>
+      </c>
+      <c r="R12" s="16">
         <v>57</v>
       </c>
-      <c r="M12" s="3">
+      <c r="S12" s="16">
+        <f t="shared" si="1"/>
+        <v>1260</v>
+      </c>
+      <c r="T12" s="3">
         <v>304</v>
       </c>
-      <c r="N12" s="3">
+      <c r="U12" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="V12" s="3">
         <v>448</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W12" s="29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>117</v>
       </c>
@@ -2102,22 +2526,51 @@
         <v>231</v>
       </c>
       <c r="J13" s="3">
+        <v>1102</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1145</v>
+      </c>
+      <c r="L13" s="3">
         <v>2247</v>
       </c>
-      <c r="K13" s="3">
+      <c r="M13" s="3">
+        <v>1148</v>
+      </c>
+      <c r="N13" s="3">
+        <v>299</v>
+      </c>
+      <c r="O13" s="3">
         <v>1447</v>
       </c>
-      <c r="L13" s="16">
+      <c r="P13" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q13" s="16">
+        <f t="shared" si="0"/>
+        <v>2250</v>
+      </c>
+      <c r="R13" s="16">
         <v>262</v>
       </c>
-      <c r="M13" s="3">
+      <c r="S13" s="16">
+        <f t="shared" si="1"/>
+        <v>3956</v>
+      </c>
+      <c r="T13" s="3">
         <v>1539</v>
       </c>
-      <c r="N13" s="3">
+      <c r="U13" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="V13" s="3">
         <v>1477</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W13" s="29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>118</v>
       </c>
@@ -2146,22 +2599,51 @@
         <v>116</v>
       </c>
       <c r="J14" s="3">
+        <v>3350</v>
+      </c>
+      <c r="K14" s="3">
+        <v>658</v>
+      </c>
+      <c r="L14" s="3">
         <v>4008</v>
       </c>
-      <c r="K14" s="3">
+      <c r="M14" s="3">
+        <v>2819</v>
+      </c>
+      <c r="N14" s="3">
+        <v>435</v>
+      </c>
+      <c r="O14" s="3">
         <v>3254</v>
       </c>
-      <c r="L14" s="16">
+      <c r="P14" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q14" s="16">
+        <f t="shared" si="0"/>
+        <v>6169</v>
+      </c>
+      <c r="R14" s="16">
         <v>216</v>
       </c>
-      <c r="M14" s="3">
+      <c r="S14" s="16">
+        <f t="shared" si="1"/>
+        <v>7478</v>
+      </c>
+      <c r="T14" s="3">
         <v>2588</v>
       </c>
-      <c r="N14" s="3">
+      <c r="U14" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="V14" s="3">
         <v>1542</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W14" s="29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>119</v>
       </c>
@@ -2190,22 +2672,51 @@
         <v>20</v>
       </c>
       <c r="J15" s="3">
+        <v>1707</v>
+      </c>
+      <c r="K15" s="3">
+        <v>509</v>
+      </c>
+      <c r="L15" s="3">
         <v>2216</v>
       </c>
-      <c r="K15" s="3">
+      <c r="M15" s="3">
+        <v>2389</v>
+      </c>
+      <c r="N15" s="3">
+        <v>325</v>
+      </c>
+      <c r="O15" s="3">
         <v>2714</v>
       </c>
-      <c r="L15" s="16">
+      <c r="P15" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q15" s="16">
+        <f t="shared" si="0"/>
+        <v>4096</v>
+      </c>
+      <c r="R15" s="16">
         <v>89</v>
       </c>
-      <c r="M15" s="3">
+      <c r="S15" s="16">
+        <f t="shared" si="1"/>
+        <v>5019</v>
+      </c>
+      <c r="T15" s="3">
         <v>2778</v>
       </c>
-      <c r="N15" s="3">
+      <c r="U15" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="V15" s="3">
         <v>618</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W15" s="29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>120</v>
       </c>
@@ -2234,22 +2745,51 @@
         <v>0</v>
       </c>
       <c r="J16" s="2">
+        <v>1775</v>
+      </c>
+      <c r="K16" s="2">
+        <v>127</v>
+      </c>
+      <c r="L16" s="2">
         <v>1902</v>
       </c>
-      <c r="K16" s="2">
+      <c r="M16" s="2">
+        <v>2090</v>
+      </c>
+      <c r="N16" s="2">
+        <v>121</v>
+      </c>
+      <c r="O16" s="2">
         <v>2211</v>
       </c>
-      <c r="L16" s="15">
+      <c r="P16" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q16" s="15">
+        <f t="shared" si="0"/>
+        <v>3865</v>
+      </c>
+      <c r="R16" s="15">
         <v>8</v>
       </c>
-      <c r="M16" s="2">
+      <c r="S16" s="15">
+        <f t="shared" si="1"/>
+        <v>4121</v>
+      </c>
+      <c r="T16" s="2">
         <v>1351</v>
       </c>
-      <c r="N16" s="2">
+      <c r="U16" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V16" s="2">
         <v>535</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W16" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>121</v>
       </c>
@@ -2278,22 +2818,51 @@
         <v>0</v>
       </c>
       <c r="J17" s="1">
+        <v>7970</v>
+      </c>
+      <c r="K17" s="1">
+        <v>2053</v>
+      </c>
+      <c r="L17" s="1">
         <v>10023</v>
       </c>
-      <c r="K17" s="1">
+      <c r="M17" s="1">
+        <v>15847</v>
+      </c>
+      <c r="N17" s="1">
+        <v>1052</v>
+      </c>
+      <c r="O17" s="1">
         <v>16899</v>
       </c>
-      <c r="L17" s="14">
+      <c r="P17" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q17" s="14">
+        <f t="shared" si="0"/>
+        <v>23817</v>
+      </c>
+      <c r="R17" s="14">
         <v>304</v>
       </c>
-      <c r="M17" s="1">
+      <c r="S17" s="14">
+        <f t="shared" si="1"/>
+        <v>27226</v>
+      </c>
+      <c r="T17" s="1">
         <v>3914</v>
       </c>
-      <c r="N17" s="1">
+      <c r="U17" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V17" s="1">
         <v>5174</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W17" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>122</v>
       </c>
@@ -2322,22 +2891,51 @@
         <v>0</v>
       </c>
       <c r="J18" s="2">
+        <v>557</v>
+      </c>
+      <c r="K18" s="2">
+        <v>220</v>
+      </c>
+      <c r="L18" s="2">
         <v>777</v>
       </c>
-      <c r="K18" s="2">
+      <c r="M18" s="2">
+        <v>1257</v>
+      </c>
+      <c r="N18" s="2">
+        <v>95</v>
+      </c>
+      <c r="O18" s="2">
         <v>1352</v>
       </c>
-      <c r="L18" s="15">
-        <v>0</v>
-      </c>
-      <c r="M18" s="2">
+      <c r="P18" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q18" s="15">
+        <f t="shared" si="0"/>
+        <v>1814</v>
+      </c>
+      <c r="R18" s="15">
+        <v>0</v>
+      </c>
+      <c r="S18" s="15">
+        <f t="shared" si="1"/>
+        <v>2129</v>
+      </c>
+      <c r="T18" s="2">
         <v>992</v>
       </c>
-      <c r="N18" s="2">
+      <c r="U18" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V18" s="2">
         <v>546</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W18" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>123</v>
       </c>
@@ -2366,22 +2964,51 @@
         <v>35</v>
       </c>
       <c r="J19" s="1">
+        <v>10601</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2683</v>
+      </c>
+      <c r="L19" s="1">
         <v>13284</v>
       </c>
-      <c r="K19" s="1">
+      <c r="M19" s="1">
+        <v>13284</v>
+      </c>
+      <c r="N19" s="1">
+        <v>875</v>
+      </c>
+      <c r="O19" s="1">
         <v>14159</v>
       </c>
-      <c r="L19" s="14">
+      <c r="P19" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q19" s="14">
+        <f t="shared" si="0"/>
+        <v>23885</v>
+      </c>
+      <c r="R19" s="14">
         <v>102</v>
       </c>
-      <c r="M19" s="1">
+      <c r="S19" s="14">
+        <f t="shared" si="1"/>
+        <v>27545</v>
+      </c>
+      <c r="T19" s="1">
         <v>3866</v>
       </c>
-      <c r="N19" s="1">
+      <c r="U19" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V19" s="1">
         <v>4293</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W19" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>124</v>
       </c>
@@ -2410,22 +3037,51 @@
         <v>0</v>
       </c>
       <c r="J20" s="2">
+        <v>267</v>
+      </c>
+      <c r="K20" s="2">
+        <v>190</v>
+      </c>
+      <c r="L20" s="2">
         <v>457</v>
       </c>
-      <c r="K20" s="2">
+      <c r="M20" s="2">
+        <v>58</v>
+      </c>
+      <c r="N20" s="2">
+        <v>2</v>
+      </c>
+      <c r="O20" s="2">
         <v>60</v>
       </c>
-      <c r="L20" s="15">
+      <c r="P20" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q20" s="15">
+        <f t="shared" si="0"/>
+        <v>325</v>
+      </c>
+      <c r="R20" s="15">
         <v>40</v>
       </c>
-      <c r="M20" s="2">
+      <c r="S20" s="15">
+        <f t="shared" si="1"/>
+        <v>557</v>
+      </c>
+      <c r="T20" s="2">
         <v>627</v>
       </c>
-      <c r="N20" s="2">
+      <c r="U20" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V20" s="2">
         <v>185</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W20" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>125</v>
       </c>
@@ -2454,22 +3110,51 @@
         <v>282</v>
       </c>
       <c r="J21" s="1">
+        <v>10889</v>
+      </c>
+      <c r="K21" s="1">
+        <v>3988</v>
+      </c>
+      <c r="L21" s="1">
         <v>14877</v>
       </c>
-      <c r="K21" s="1">
+      <c r="M21" s="1">
+        <v>10779</v>
+      </c>
+      <c r="N21" s="1">
+        <v>1418</v>
+      </c>
+      <c r="O21" s="1">
         <v>12197</v>
       </c>
-      <c r="L21" s="14">
+      <c r="P21" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q21" s="14">
+        <f t="shared" si="0"/>
+        <v>21668</v>
+      </c>
+      <c r="R21" s="14">
         <v>350</v>
       </c>
-      <c r="M21" s="1">
+      <c r="S21" s="14">
+        <f t="shared" si="1"/>
+        <v>27424</v>
+      </c>
+      <c r="T21" s="1">
         <v>3099</v>
       </c>
-      <c r="N21" s="1">
+      <c r="U21" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V21" s="1">
         <v>4782</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W21" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>126</v>
       </c>
@@ -2498,22 +3183,51 @@
         <v>9</v>
       </c>
       <c r="J22" s="2">
+        <v>1107</v>
+      </c>
+      <c r="K22" s="2">
+        <v>300</v>
+      </c>
+      <c r="L22" s="2">
         <v>1407</v>
       </c>
-      <c r="K22" s="2">
+      <c r="M22" s="2">
+        <v>525</v>
+      </c>
+      <c r="N22" s="2">
+        <v>23</v>
+      </c>
+      <c r="O22" s="2">
         <v>548</v>
       </c>
-      <c r="L22" s="15">
+      <c r="P22" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q22" s="15">
+        <f t="shared" si="0"/>
+        <v>1632</v>
+      </c>
+      <c r="R22" s="15">
         <v>42</v>
       </c>
-      <c r="M22" s="2">
+      <c r="S22" s="15">
+        <f t="shared" si="1"/>
+        <v>1997</v>
+      </c>
+      <c r="T22" s="2">
         <v>1099</v>
       </c>
-      <c r="N22" s="2">
+      <c r="U22" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V22" s="2">
         <v>335</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W22" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>127</v>
       </c>
@@ -2542,22 +3256,51 @@
         <v>0</v>
       </c>
       <c r="J23" s="1">
+        <v>10265</v>
+      </c>
+      <c r="K23" s="1">
+        <v>2685</v>
+      </c>
+      <c r="L23" s="1">
         <v>12950</v>
       </c>
-      <c r="K23" s="1">
+      <c r="M23" s="1">
+        <v>15551</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1248</v>
+      </c>
+      <c r="O23" s="1">
         <v>16799</v>
       </c>
-      <c r="L23" s="14">
+      <c r="P23" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q23" s="14">
+        <f t="shared" si="0"/>
+        <v>25816</v>
+      </c>
+      <c r="R23" s="14">
         <v>853</v>
       </c>
-      <c r="M23" s="1">
+      <c r="S23" s="14">
+        <f t="shared" si="1"/>
+        <v>30602</v>
+      </c>
+      <c r="T23" s="1">
         <v>3090</v>
       </c>
-      <c r="N23" s="1">
+      <c r="U23" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V23" s="1">
         <v>5685</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W23" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>128</v>
       </c>
@@ -2586,22 +3329,51 @@
         <v>0</v>
       </c>
       <c r="J24" s="2">
+        <v>36195</v>
+      </c>
+      <c r="K24" s="2">
+        <v>20059</v>
+      </c>
+      <c r="L24" s="2">
         <v>56254</v>
       </c>
-      <c r="K24" s="2">
+      <c r="M24" s="2">
+        <v>56165</v>
+      </c>
+      <c r="N24" s="2">
+        <v>6609</v>
+      </c>
+      <c r="O24" s="2">
         <v>62774</v>
       </c>
-      <c r="L24" s="15">
+      <c r="P24" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q24" s="15">
+        <f t="shared" si="0"/>
+        <v>92360</v>
+      </c>
+      <c r="R24" s="15">
         <v>2708</v>
       </c>
-      <c r="M24" s="2">
+      <c r="S24" s="15">
+        <f t="shared" si="1"/>
+        <v>121736</v>
+      </c>
+      <c r="T24" s="2">
         <v>10493</v>
       </c>
-      <c r="N24" s="2">
+      <c r="U24" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V24" s="2">
         <v>13846</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W24" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>129</v>
       </c>
@@ -2630,22 +3402,51 @@
         <v>0</v>
       </c>
       <c r="J25" s="1">
+        <v>2578</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1105</v>
+      </c>
+      <c r="L25" s="1">
         <v>3683</v>
       </c>
-      <c r="K25" s="1">
+      <c r="M25" s="1">
+        <v>4578</v>
+      </c>
+      <c r="N25" s="1">
+        <v>802</v>
+      </c>
+      <c r="O25" s="1">
         <v>5380</v>
       </c>
-      <c r="L25" s="14">
+      <c r="P25" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q25" s="14">
+        <f t="shared" si="0"/>
+        <v>7156</v>
+      </c>
+      <c r="R25" s="14">
         <v>318</v>
       </c>
-      <c r="M25" s="1">
+      <c r="S25" s="14">
+        <f t="shared" si="1"/>
+        <v>9381</v>
+      </c>
+      <c r="T25" s="1">
         <v>3716</v>
       </c>
-      <c r="N25" s="1">
+      <c r="U25" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V25" s="1">
         <v>1335</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W25" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>130</v>
       </c>
@@ -2679,7 +3480,7 @@
       <c r="K26" s="2">
         <v>0</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="2">
         <v>0</v>
       </c>
       <c r="M26" s="2">
@@ -2688,8 +3489,37 @@
       <c r="N26" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q26" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="15">
+        <v>0</v>
+      </c>
+      <c r="S26" s="15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0</v>
+      </c>
+      <c r="U26" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V26" s="2">
+        <v>0</v>
+      </c>
+      <c r="W26" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>131</v>
       </c>
@@ -2718,22 +3548,51 @@
         <v>0</v>
       </c>
       <c r="J27" s="1">
+        <v>3727</v>
+      </c>
+      <c r="K27" s="1">
+        <v>987</v>
+      </c>
+      <c r="L27" s="1">
         <v>4714</v>
       </c>
-      <c r="K27" s="1">
+      <c r="M27" s="1">
+        <v>2929</v>
+      </c>
+      <c r="N27" s="1">
+        <v>366</v>
+      </c>
+      <c r="O27" s="1">
         <v>3295</v>
       </c>
-      <c r="L27" s="14">
+      <c r="P27" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q27" s="14">
+        <f t="shared" si="0"/>
+        <v>6656</v>
+      </c>
+      <c r="R27" s="14">
         <v>223</v>
       </c>
-      <c r="M27" s="1">
+      <c r="S27" s="14">
+        <f t="shared" si="1"/>
+        <v>8232</v>
+      </c>
+      <c r="T27" s="1">
         <v>1898</v>
       </c>
-      <c r="N27" s="1">
+      <c r="U27" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V27" s="1">
         <v>2033</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W27" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>132</v>
       </c>
@@ -2762,22 +3621,51 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
+        <v>1060</v>
+      </c>
+      <c r="K28" s="2">
+        <v>341</v>
+      </c>
+      <c r="L28" s="2">
         <v>1401</v>
       </c>
-      <c r="K28" s="2">
+      <c r="M28" s="2">
+        <v>2142</v>
+      </c>
+      <c r="N28" s="2">
+        <v>204</v>
+      </c>
+      <c r="O28" s="2">
         <v>2346</v>
       </c>
-      <c r="L28" s="15">
+      <c r="P28" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q28" s="15">
+        <f t="shared" si="0"/>
+        <v>3202</v>
+      </c>
+      <c r="R28" s="15">
         <v>35</v>
       </c>
-      <c r="M28" s="2">
+      <c r="S28" s="15">
+        <f t="shared" si="1"/>
+        <v>3782</v>
+      </c>
+      <c r="T28" s="2">
         <v>863</v>
       </c>
-      <c r="N28" s="2">
+      <c r="U28" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V28" s="2">
         <v>789</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W28" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>133</v>
       </c>
@@ -2806,22 +3694,51 @@
         <v>237</v>
       </c>
       <c r="J29" s="1">
+        <v>7050</v>
+      </c>
+      <c r="K29" s="1">
+        <v>1672</v>
+      </c>
+      <c r="L29" s="1">
         <v>8722</v>
       </c>
-      <c r="K29" s="1">
+      <c r="M29" s="1">
+        <v>13055</v>
+      </c>
+      <c r="N29" s="1">
+        <v>1275</v>
+      </c>
+      <c r="O29" s="1">
         <v>14330</v>
       </c>
-      <c r="L29" s="14">
+      <c r="P29" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q29" s="14">
+        <f t="shared" si="0"/>
+        <v>20105</v>
+      </c>
+      <c r="R29" s="14">
         <v>310</v>
       </c>
-      <c r="M29" s="1">
+      <c r="S29" s="14">
+        <f t="shared" si="1"/>
+        <v>23362</v>
+      </c>
+      <c r="T29" s="1">
         <v>4144</v>
       </c>
-      <c r="N29" s="1">
+      <c r="U29" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V29" s="1">
         <v>4695</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W29" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>134</v>
       </c>
@@ -2850,22 +3767,51 @@
         <v>0</v>
       </c>
       <c r="J30" s="2">
+        <v>486</v>
+      </c>
+      <c r="K30" s="2">
+        <v>12</v>
+      </c>
+      <c r="L30" s="2">
         <v>498</v>
       </c>
-      <c r="K30" s="2">
+      <c r="M30" s="2">
+        <v>200</v>
+      </c>
+      <c r="N30" s="2">
+        <v>2</v>
+      </c>
+      <c r="O30" s="2">
         <v>202</v>
       </c>
-      <c r="L30" s="15">
+      <c r="P30" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q30" s="15">
+        <f t="shared" si="0"/>
+        <v>686</v>
+      </c>
+      <c r="R30" s="15">
         <v>5</v>
       </c>
-      <c r="M30" s="2">
+      <c r="S30" s="15">
+        <f t="shared" si="1"/>
+        <v>705</v>
+      </c>
+      <c r="T30" s="2">
         <v>168</v>
       </c>
-      <c r="N30" s="2">
+      <c r="U30" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V30" s="2">
         <v>435</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W30" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>135</v>
       </c>
@@ -2894,22 +3840,51 @@
         <v>0</v>
       </c>
       <c r="J31" s="1">
+        <v>1270</v>
+      </c>
+      <c r="K31" s="1">
+        <v>525</v>
+      </c>
+      <c r="L31" s="1">
         <v>1795</v>
       </c>
-      <c r="K31" s="1">
+      <c r="M31" s="1">
+        <v>2176</v>
+      </c>
+      <c r="N31" s="1">
+        <v>335</v>
+      </c>
+      <c r="O31" s="1">
         <v>2511</v>
       </c>
-      <c r="L31" s="14">
+      <c r="P31" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q31" s="14">
+        <f t="shared" si="0"/>
+        <v>3446</v>
+      </c>
+      <c r="R31" s="14">
         <v>183</v>
       </c>
-      <c r="M31" s="1">
+      <c r="S31" s="14">
+        <f t="shared" si="1"/>
+        <v>4489</v>
+      </c>
+      <c r="T31" s="1">
         <v>2568</v>
       </c>
-      <c r="N31" s="1">
+      <c r="U31" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V31" s="1">
         <v>477</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W31" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>136</v>
       </c>
@@ -2938,22 +3913,51 @@
         <v>0</v>
       </c>
       <c r="J32" s="2">
+        <v>8702</v>
+      </c>
+      <c r="K32" s="2">
+        <v>4287</v>
+      </c>
+      <c r="L32" s="2">
         <v>12989</v>
       </c>
-      <c r="K32" s="2">
+      <c r="M32" s="2">
+        <v>5726</v>
+      </c>
+      <c r="N32" s="2">
+        <v>990</v>
+      </c>
+      <c r="O32" s="2">
         <v>6716</v>
       </c>
-      <c r="L32" s="15">
+      <c r="P32" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q32" s="15">
+        <f t="shared" si="0"/>
+        <v>14428</v>
+      </c>
+      <c r="R32" s="15">
         <v>2139</v>
       </c>
-      <c r="M32" s="2">
+      <c r="S32" s="15">
+        <f t="shared" si="1"/>
+        <v>21844</v>
+      </c>
+      <c r="T32" s="2">
         <v>5266</v>
       </c>
-      <c r="N32" s="2">
+      <c r="U32" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V32" s="2">
         <v>4470</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W32" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>137</v>
       </c>
@@ -2982,22 +3986,51 @@
         <v>10</v>
       </c>
       <c r="J33" s="1">
+        <v>6966</v>
+      </c>
+      <c r="K33" s="1">
+        <v>1688</v>
+      </c>
+      <c r="L33" s="1">
         <v>8654</v>
       </c>
-      <c r="K33" s="1">
+      <c r="M33" s="1">
+        <v>7994</v>
+      </c>
+      <c r="N33" s="1">
+        <v>684</v>
+      </c>
+      <c r="O33" s="1">
         <v>8678</v>
       </c>
-      <c r="L33" s="14">
+      <c r="P33" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q33" s="14">
+        <f t="shared" si="0"/>
+        <v>14960</v>
+      </c>
+      <c r="R33" s="14">
         <v>121</v>
       </c>
-      <c r="M33" s="1">
+      <c r="S33" s="14">
+        <f t="shared" si="1"/>
+        <v>17453</v>
+      </c>
+      <c r="T33" s="1">
         <v>5030</v>
       </c>
-      <c r="N33" s="1">
+      <c r="U33" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V33" s="1">
         <v>3214</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W33" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>138</v>
       </c>
@@ -3026,22 +4059,51 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
+        <v>3448</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1079</v>
+      </c>
+      <c r="L34" s="2">
         <v>4527</v>
       </c>
-      <c r="K34" s="2">
+      <c r="M34" s="2">
+        <v>2356</v>
+      </c>
+      <c r="N34" s="2">
+        <v>288</v>
+      </c>
+      <c r="O34" s="2">
         <v>2644</v>
       </c>
-      <c r="L34" s="15">
+      <c r="P34" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q34" s="15">
+        <f t="shared" si="0"/>
+        <v>5804</v>
+      </c>
+      <c r="R34" s="15">
         <v>713</v>
       </c>
-      <c r="M34" s="2">
+      <c r="S34" s="15">
+        <f t="shared" si="1"/>
+        <v>7884</v>
+      </c>
+      <c r="T34" s="2">
         <v>1011</v>
       </c>
-      <c r="N34" s="2">
+      <c r="U34" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V34" s="2">
         <v>1623</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W34" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>139</v>
       </c>
@@ -3070,22 +4132,51 @@
         <v>0</v>
       </c>
       <c r="J35" s="1">
+        <v>26979</v>
+      </c>
+      <c r="K35" s="1">
+        <v>7151</v>
+      </c>
+      <c r="L35" s="1">
         <v>34130</v>
       </c>
-      <c r="K35" s="1">
+      <c r="M35" s="1">
+        <v>47549</v>
+      </c>
+      <c r="N35" s="1">
+        <v>4039</v>
+      </c>
+      <c r="O35" s="1">
         <v>51588</v>
       </c>
-      <c r="L35" s="14">
+      <c r="P35" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q35" s="14">
+        <f t="shared" si="0"/>
+        <v>74528</v>
+      </c>
+      <c r="R35" s="14">
         <v>1956</v>
       </c>
-      <c r="M35" s="1">
+      <c r="S35" s="14">
+        <f t="shared" si="1"/>
+        <v>87674</v>
+      </c>
+      <c r="T35" s="1">
         <v>10138</v>
       </c>
-      <c r="N35" s="1">
+      <c r="U35" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V35" s="1">
         <v>8585</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W35" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>140</v>
       </c>
@@ -3114,22 +4205,51 @@
         <v>0</v>
       </c>
       <c r="J36" s="2">
+        <v>4104</v>
+      </c>
+      <c r="K36" s="2">
+        <v>2915</v>
+      </c>
+      <c r="L36" s="2">
         <v>7019</v>
       </c>
-      <c r="K36" s="2">
+      <c r="M36" s="2">
+        <v>4270</v>
+      </c>
+      <c r="N36" s="2">
+        <v>846</v>
+      </c>
+      <c r="O36" s="2">
         <v>5116</v>
       </c>
-      <c r="L36" s="15">
+      <c r="P36" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q36" s="15">
+        <f t="shared" si="0"/>
+        <v>8374</v>
+      </c>
+      <c r="R36" s="15">
         <v>184</v>
       </c>
-      <c r="M36" s="2">
+      <c r="S36" s="15">
+        <f t="shared" si="1"/>
+        <v>12319</v>
+      </c>
+      <c r="T36" s="2">
         <v>4635</v>
       </c>
-      <c r="N36" s="2">
+      <c r="U36" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V36" s="2">
         <v>1668</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W36" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>141</v>
       </c>
@@ -3158,22 +4278,51 @@
         <v>506</v>
       </c>
       <c r="J37" s="1">
+        <v>11542</v>
+      </c>
+      <c r="K37" s="1">
+        <v>3708</v>
+      </c>
+      <c r="L37" s="1">
         <v>15250</v>
       </c>
-      <c r="K37" s="1">
+      <c r="M37" s="1">
+        <v>21620</v>
+      </c>
+      <c r="N37" s="1">
+        <v>1190</v>
+      </c>
+      <c r="O37" s="1">
         <v>22810</v>
       </c>
-      <c r="L37" s="14">
+      <c r="P37" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q37" s="14">
+        <f t="shared" si="0"/>
+        <v>33162</v>
+      </c>
+      <c r="R37" s="14">
         <v>4754</v>
       </c>
-      <c r="M37" s="1">
+      <c r="S37" s="14">
+        <f t="shared" si="1"/>
+        <v>42814</v>
+      </c>
+      <c r="T37" s="1">
         <v>3038</v>
       </c>
-      <c r="N37" s="1">
+      <c r="U37" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V37" s="1">
         <v>4102</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W37" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>142</v>
       </c>
@@ -3202,22 +4351,51 @@
         <v>0</v>
       </c>
       <c r="J38" s="2">
+        <v>720</v>
+      </c>
+      <c r="K38" s="2">
+        <v>18</v>
+      </c>
+      <c r="L38" s="2">
         <v>738</v>
       </c>
-      <c r="K38" s="2">
+      <c r="M38" s="2">
+        <v>1118</v>
+      </c>
+      <c r="N38" s="2">
+        <v>20</v>
+      </c>
+      <c r="O38" s="2">
         <v>1138</v>
       </c>
-      <c r="L38" s="15">
-        <v>0</v>
-      </c>
-      <c r="M38" s="2">
+      <c r="P38" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q38" s="15">
+        <f t="shared" si="0"/>
+        <v>1838</v>
+      </c>
+      <c r="R38" s="15">
+        <v>0</v>
+      </c>
+      <c r="S38" s="15">
+        <f t="shared" si="1"/>
+        <v>1876</v>
+      </c>
+      <c r="T38" s="2">
         <v>1660</v>
       </c>
-      <c r="N38" s="2">
+      <c r="U38" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V38" s="2">
         <v>308</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W38" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>143</v>
       </c>
@@ -3246,22 +4424,51 @@
         <v>0</v>
       </c>
       <c r="J39" s="1">
+        <v>393</v>
+      </c>
+      <c r="K39" s="1">
+        <v>161</v>
+      </c>
+      <c r="L39" s="1">
         <v>554</v>
       </c>
-      <c r="K39" s="1">
+      <c r="M39" s="1">
+        <v>1504</v>
+      </c>
+      <c r="N39" s="1">
+        <v>84</v>
+      </c>
+      <c r="O39" s="1">
         <v>1588</v>
       </c>
-      <c r="L39" s="14">
+      <c r="P39" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q39" s="14">
+        <f t="shared" si="0"/>
+        <v>1897</v>
+      </c>
+      <c r="R39" s="14">
         <v>19</v>
       </c>
-      <c r="M39" s="1">
+      <c r="S39" s="14">
+        <f t="shared" si="1"/>
+        <v>2161</v>
+      </c>
+      <c r="T39" s="1">
         <v>811</v>
       </c>
-      <c r="N39" s="1">
+      <c r="U39" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V39" s="1">
         <v>859</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W39" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>144</v>
       </c>
@@ -3290,22 +4497,51 @@
         <v>0</v>
       </c>
       <c r="J40" s="5">
+        <v>88</v>
+      </c>
+      <c r="K40" s="5">
+        <v>4</v>
+      </c>
+      <c r="L40" s="5">
         <v>92</v>
       </c>
-      <c r="K40" s="5">
+      <c r="M40" s="5">
+        <v>3961</v>
+      </c>
+      <c r="N40" s="5">
+        <v>1</v>
+      </c>
+      <c r="O40" s="5">
         <v>3962</v>
       </c>
-      <c r="L40" s="18">
+      <c r="P40" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q40" s="18">
+        <f t="shared" si="0"/>
+        <v>4049</v>
+      </c>
+      <c r="R40" s="18">
         <v>4</v>
       </c>
-      <c r="M40" s="5">
+      <c r="S40" s="18">
+        <f t="shared" si="1"/>
+        <v>4058</v>
+      </c>
+      <c r="T40" s="5">
         <v>874</v>
       </c>
-      <c r="N40" s="5">
+      <c r="U40" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="V40" s="5">
         <v>178</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W40" s="30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>145</v>
       </c>
@@ -3334,22 +4570,51 @@
         <v>0</v>
       </c>
       <c r="J41" s="5">
+        <v>50</v>
+      </c>
+      <c r="K41" s="5">
+        <v>11</v>
+      </c>
+      <c r="L41" s="5">
         <v>61</v>
       </c>
-      <c r="K41" s="5">
+      <c r="M41" s="5">
         <v>17846</v>
       </c>
-      <c r="L41" s="18">
+      <c r="N41" s="5">
+        <v>0</v>
+      </c>
+      <c r="O41" s="5">
+        <v>17846</v>
+      </c>
+      <c r="P41" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q41" s="18">
+        <f t="shared" si="0"/>
+        <v>17896</v>
+      </c>
+      <c r="R41" s="18">
         <v>27</v>
       </c>
-      <c r="M41" s="5">
+      <c r="S41" s="18">
+        <f t="shared" si="1"/>
+        <v>17934</v>
+      </c>
+      <c r="T41" s="5">
         <v>866</v>
       </c>
-      <c r="N41" s="5">
+      <c r="U41" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="V41" s="5">
         <v>505</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W41" s="30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>146</v>
       </c>
@@ -3381,19 +4646,48 @@
         <v>364</v>
       </c>
       <c r="K42" s="5">
+        <v>0</v>
+      </c>
+      <c r="L42" s="5">
+        <v>364</v>
+      </c>
+      <c r="M42" s="5">
         <v>50</v>
       </c>
-      <c r="L42" s="18">
-        <v>0</v>
-      </c>
-      <c r="M42" s="5">
+      <c r="N42" s="5">
+        <v>0</v>
+      </c>
+      <c r="O42" s="5">
+        <v>50</v>
+      </c>
+      <c r="P42" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q42" s="18">
+        <f t="shared" si="0"/>
+        <v>414</v>
+      </c>
+      <c r="R42" s="18">
+        <v>0</v>
+      </c>
+      <c r="S42" s="18">
+        <f t="shared" si="1"/>
+        <v>414</v>
+      </c>
+      <c r="T42" s="5">
         <v>303</v>
       </c>
-      <c r="N42" s="5">
+      <c r="U42" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="V42" s="5">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W42" s="30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>147</v>
       </c>
@@ -3425,19 +4719,48 @@
         <v>25</v>
       </c>
       <c r="K43" s="5">
+        <v>0</v>
+      </c>
+      <c r="L43" s="5">
+        <v>25</v>
+      </c>
+      <c r="M43" s="5">
         <v>1304</v>
       </c>
-      <c r="L43" s="18">
-        <v>0</v>
-      </c>
-      <c r="M43" s="5">
+      <c r="N43" s="5">
+        <v>0</v>
+      </c>
+      <c r="O43" s="5">
+        <v>1304</v>
+      </c>
+      <c r="P43" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q43" s="18">
+        <f t="shared" si="0"/>
+        <v>1329</v>
+      </c>
+      <c r="R43" s="18">
+        <v>0</v>
+      </c>
+      <c r="S43" s="18">
+        <f t="shared" si="1"/>
+        <v>1329</v>
+      </c>
+      <c r="T43" s="5">
         <v>250</v>
       </c>
-      <c r="N43" s="5">
+      <c r="U43" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="V43" s="5">
         <v>96</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W43" s="30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>148</v>
       </c>
@@ -3471,7 +4794,7 @@
       <c r="K44" s="5">
         <v>0</v>
       </c>
-      <c r="L44" s="18">
+      <c r="L44" s="5">
         <v>0</v>
       </c>
       <c r="M44" s="5">
@@ -3480,8 +4803,37 @@
       <c r="N44" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="5">
+        <v>0</v>
+      </c>
+      <c r="P44" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q44" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R44" s="18">
+        <v>0</v>
+      </c>
+      <c r="S44" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T44" s="5">
+        <v>0</v>
+      </c>
+      <c r="U44" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="V44" s="5">
+        <v>0</v>
+      </c>
+      <c r="W44" s="30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>149</v>
       </c>
@@ -3510,22 +4862,51 @@
         <v>0</v>
       </c>
       <c r="J45" s="1">
+        <v>1367</v>
+      </c>
+      <c r="K45" s="1">
+        <v>962</v>
+      </c>
+      <c r="L45" s="1">
         <v>2329</v>
       </c>
-      <c r="K45" s="1">
+      <c r="M45" s="1">
+        <v>1267</v>
+      </c>
+      <c r="N45" s="1">
+        <v>153</v>
+      </c>
+      <c r="O45" s="1">
         <v>1420</v>
       </c>
-      <c r="L45" s="14">
+      <c r="P45" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q45" s="14">
+        <f t="shared" si="0"/>
+        <v>2634</v>
+      </c>
+      <c r="R45" s="14">
         <v>1433</v>
       </c>
-      <c r="M45" s="1">
+      <c r="S45" s="14">
+        <f t="shared" si="1"/>
+        <v>5182</v>
+      </c>
+      <c r="T45" s="1">
         <v>1683</v>
       </c>
-      <c r="N45" s="1">
+      <c r="U45" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V45" s="1">
         <v>645</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W45" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
         <v>150</v>
       </c>
@@ -3554,22 +4935,51 @@
         <v>0</v>
       </c>
       <c r="J46" s="2">
+        <v>5806</v>
+      </c>
+      <c r="K46" s="2">
+        <v>3396</v>
+      </c>
+      <c r="L46" s="2">
         <v>9202</v>
       </c>
-      <c r="K46" s="2">
+      <c r="M46" s="2">
+        <v>9840</v>
+      </c>
+      <c r="N46" s="2">
+        <v>2377</v>
+      </c>
+      <c r="O46" s="2">
         <v>12217</v>
       </c>
-      <c r="L46" s="15">
+      <c r="P46" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q46" s="15">
+        <f t="shared" si="0"/>
+        <v>15646</v>
+      </c>
+      <c r="R46" s="15">
         <v>66</v>
       </c>
-      <c r="M46" s="2">
+      <c r="S46" s="15">
+        <f t="shared" si="1"/>
+        <v>21485</v>
+      </c>
+      <c r="T46" s="2">
         <v>5312</v>
       </c>
-      <c r="N46" s="2">
+      <c r="U46" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V46" s="2">
         <v>4178</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W46" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>151</v>
       </c>
@@ -3598,22 +5008,51 @@
         <v>480</v>
       </c>
       <c r="J47" s="1">
+        <v>9606</v>
+      </c>
+      <c r="K47" s="1">
+        <v>2339</v>
+      </c>
+      <c r="L47" s="1">
         <v>11945</v>
       </c>
-      <c r="K47" s="1">
+      <c r="M47" s="1">
+        <v>36478</v>
+      </c>
+      <c r="N47" s="1">
+        <v>2265</v>
+      </c>
+      <c r="O47" s="1">
         <v>38743</v>
       </c>
-      <c r="L47" s="14">
+      <c r="P47" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q47" s="14">
+        <f t="shared" si="0"/>
+        <v>46084</v>
+      </c>
+      <c r="R47" s="14">
         <v>792</v>
       </c>
-      <c r="M47" s="1">
+      <c r="S47" s="14">
+        <f t="shared" si="1"/>
+        <v>51480</v>
+      </c>
+      <c r="T47" s="1">
         <v>5320</v>
       </c>
-      <c r="N47" s="1">
+      <c r="U47" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V47" s="1">
         <v>7745</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W47" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>152</v>
       </c>
@@ -3642,22 +5081,51 @@
         <v>126</v>
       </c>
       <c r="J48" s="2">
+        <v>6899</v>
+      </c>
+      <c r="K48" s="2">
+        <v>2096</v>
+      </c>
+      <c r="L48" s="2">
         <v>8995</v>
       </c>
-      <c r="K48" s="2">
+      <c r="M48" s="2">
+        <v>13612</v>
+      </c>
+      <c r="N48" s="2">
+        <v>1165</v>
+      </c>
+      <c r="O48" s="2">
         <v>14777</v>
       </c>
-      <c r="L48" s="15">
+      <c r="P48" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q48" s="15">
+        <f t="shared" si="0"/>
+        <v>20511</v>
+      </c>
+      <c r="R48" s="15">
         <v>142</v>
       </c>
-      <c r="M48" s="2">
+      <c r="S48" s="15">
+        <f t="shared" si="1"/>
+        <v>23914</v>
+      </c>
+      <c r="T48" s="2">
         <v>5318</v>
       </c>
-      <c r="N48" s="2">
+      <c r="U48" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V48" s="2">
         <v>2165</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W48" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>153</v>
       </c>
@@ -3686,22 +5154,51 @@
         <v>155</v>
       </c>
       <c r="J49" s="1">
+        <v>4432</v>
+      </c>
+      <c r="K49" s="1">
+        <v>1638</v>
+      </c>
+      <c r="L49" s="1">
         <v>6070</v>
       </c>
-      <c r="K49" s="1">
+      <c r="M49" s="1">
+        <v>11489</v>
+      </c>
+      <c r="N49" s="1">
+        <v>1206</v>
+      </c>
+      <c r="O49" s="1">
         <v>12695</v>
       </c>
-      <c r="L49" s="14">
+      <c r="P49" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q49" s="14">
+        <f t="shared" si="0"/>
+        <v>15921</v>
+      </c>
+      <c r="R49" s="14">
         <v>562</v>
       </c>
-      <c r="M49" s="1">
+      <c r="S49" s="14">
+        <f t="shared" si="1"/>
+        <v>19327</v>
+      </c>
+      <c r="T49" s="1">
         <v>2384</v>
       </c>
-      <c r="N49" s="1">
+      <c r="U49" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V49" s="1">
         <v>4318</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W49" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>154</v>
       </c>
@@ -3730,22 +5227,51 @@
         <v>0</v>
       </c>
       <c r="J50" s="2">
+        <v>17740</v>
+      </c>
+      <c r="K50" s="2">
+        <v>4210</v>
+      </c>
+      <c r="L50" s="2">
         <v>21950</v>
       </c>
-      <c r="K50" s="2">
+      <c r="M50" s="2">
+        <v>23074</v>
+      </c>
+      <c r="N50" s="2">
+        <v>1684</v>
+      </c>
+      <c r="O50" s="2">
         <v>24758</v>
       </c>
-      <c r="L50" s="15">
+      <c r="P50" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q50" s="15">
+        <f t="shared" si="0"/>
+        <v>40814</v>
+      </c>
+      <c r="R50" s="15">
         <v>3481</v>
       </c>
-      <c r="M50" s="2">
+      <c r="S50" s="15">
+        <f t="shared" si="1"/>
+        <v>50189</v>
+      </c>
+      <c r="T50" s="2">
         <v>4867</v>
       </c>
-      <c r="N50" s="2">
+      <c r="U50" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V50" s="2">
         <v>7995</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W50" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>155</v>
       </c>
@@ -3774,22 +5300,51 @@
         <v>50</v>
       </c>
       <c r="J51" s="1">
+        <v>3009</v>
+      </c>
+      <c r="K51" s="1">
+        <v>868</v>
+      </c>
+      <c r="L51" s="1">
         <v>3877</v>
       </c>
-      <c r="K51" s="1">
+      <c r="M51" s="1">
+        <v>3695</v>
+      </c>
+      <c r="N51" s="1">
+        <v>531</v>
+      </c>
+      <c r="O51" s="1">
         <v>4226</v>
       </c>
-      <c r="L51" s="14">
+      <c r="P51" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q51" s="14">
+        <f t="shared" si="0"/>
+        <v>6704</v>
+      </c>
+      <c r="R51" s="14">
         <v>58</v>
       </c>
-      <c r="M51" s="1">
+      <c r="S51" s="14">
+        <f t="shared" si="1"/>
+        <v>8161</v>
+      </c>
+      <c r="T51" s="1">
         <v>1564</v>
       </c>
-      <c r="N51" s="1">
+      <c r="U51" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V51" s="1">
         <v>1974</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W51" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>156</v>
       </c>
@@ -3818,22 +5373,51 @@
         <v>0</v>
       </c>
       <c r="J52" s="2">
+        <v>5292</v>
+      </c>
+      <c r="K52" s="2">
+        <v>1288</v>
+      </c>
+      <c r="L52" s="2">
         <v>6580</v>
       </c>
-      <c r="K52" s="2">
+      <c r="M52" s="2">
+        <v>8755</v>
+      </c>
+      <c r="N52" s="2">
+        <v>1346</v>
+      </c>
+      <c r="O52" s="2">
         <v>10101</v>
       </c>
-      <c r="L52" s="15">
+      <c r="P52" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q52" s="15">
+        <f t="shared" si="0"/>
+        <v>14047</v>
+      </c>
+      <c r="R52" s="15">
         <v>205</v>
       </c>
-      <c r="M52" s="2">
+      <c r="S52" s="15">
+        <f t="shared" si="1"/>
+        <v>16886</v>
+      </c>
+      <c r="T52" s="2">
         <v>3361</v>
       </c>
-      <c r="N52" s="2">
+      <c r="U52" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V52" s="2">
         <v>2833</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W52" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>157</v>
       </c>
@@ -3862,22 +5446,51 @@
         <v>0</v>
       </c>
       <c r="J53" s="1">
+        <v>974</v>
+      </c>
+      <c r="K53" s="1">
+        <v>952</v>
+      </c>
+      <c r="L53" s="1">
         <v>1926</v>
       </c>
-      <c r="K53" s="1">
+      <c r="M53" s="1">
+        <v>1383</v>
+      </c>
+      <c r="N53" s="1">
+        <v>195</v>
+      </c>
+      <c r="O53" s="1">
         <v>1578</v>
       </c>
-      <c r="L53" s="14">
+      <c r="P53" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q53" s="14">
+        <f t="shared" si="0"/>
+        <v>2357</v>
+      </c>
+      <c r="R53" s="14">
         <v>33</v>
       </c>
-      <c r="M53" s="1">
+      <c r="S53" s="14">
+        <f t="shared" si="1"/>
+        <v>3537</v>
+      </c>
+      <c r="T53" s="1">
         <v>2075</v>
       </c>
-      <c r="N53" s="1">
+      <c r="U53" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V53" s="1">
         <v>1440</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W53" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>158</v>
       </c>
@@ -3906,22 +5519,51 @@
         <v>0</v>
       </c>
       <c r="J54" s="2">
+        <v>1120</v>
+      </c>
+      <c r="K54" s="2">
+        <v>419</v>
+      </c>
+      <c r="L54" s="2">
         <v>1539</v>
       </c>
-      <c r="K54" s="2">
+      <c r="M54" s="2">
+        <v>1581</v>
+      </c>
+      <c r="N54" s="2">
+        <v>206</v>
+      </c>
+      <c r="O54" s="2">
         <v>1787</v>
       </c>
-      <c r="L54" s="15">
+      <c r="P54" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q54" s="15">
+        <f t="shared" si="0"/>
+        <v>2701</v>
+      </c>
+      <c r="R54" s="15">
         <v>16</v>
       </c>
-      <c r="M54" s="2">
+      <c r="S54" s="15">
+        <f t="shared" si="1"/>
+        <v>3342</v>
+      </c>
+      <c r="T54" s="2">
         <v>2146</v>
       </c>
-      <c r="N54" s="2">
+      <c r="U54" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="V54" s="2">
         <v>245</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W54" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>159</v>
       </c>
@@ -3950,22 +5592,51 @@
         <v>0</v>
       </c>
       <c r="J55" s="1">
+        <v>2347</v>
+      </c>
+      <c r="K55" s="1">
+        <v>262</v>
+      </c>
+      <c r="L55" s="1">
         <v>2609</v>
       </c>
-      <c r="K55" s="1">
+      <c r="M55" s="1">
+        <v>5273</v>
+      </c>
+      <c r="N55" s="1">
+        <v>568</v>
+      </c>
+      <c r="O55" s="1">
         <v>5841</v>
       </c>
-      <c r="L55" s="14">
+      <c r="P55" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q55" s="14">
+        <f t="shared" si="0"/>
+        <v>7620</v>
+      </c>
+      <c r="R55" s="14">
         <v>11</v>
       </c>
-      <c r="M55" s="1">
+      <c r="S55" s="14">
+        <f t="shared" si="1"/>
+        <v>8461</v>
+      </c>
+      <c r="T55" s="1">
         <v>1714</v>
       </c>
-      <c r="N55" s="1">
+      <c r="U55" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="V55" s="1">
         <v>3383</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W55" s="27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>160</v>
       </c>
@@ -3974,55 +5645,88 @@
         <v>2520</v>
       </c>
       <c r="C56" s="20">
-        <f t="shared" ref="C56:N56" si="0">SUM(C12:C15)</f>
+        <f t="shared" ref="C56:V56" si="2">SUM(C12:C15)</f>
         <v>18905</v>
       </c>
       <c r="D56" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2507</v>
       </c>
       <c r="E56" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1890</v>
       </c>
       <c r="F56" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>558</v>
       </c>
       <c r="G56" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5288</v>
       </c>
       <c r="H56" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>773</v>
       </c>
       <c r="I56" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>409</v>
       </c>
       <c r="J56" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J56:K56" si="3">SUM(J12:J15)</f>
+        <v>6564</v>
+      </c>
+      <c r="K56" s="20">
+        <f t="shared" si="3"/>
+        <v>2552</v>
+      </c>
+      <c r="L56" s="20">
+        <f t="shared" si="2"/>
         <v>9116</v>
       </c>
-      <c r="K56" s="20">
-        <f t="shared" si="0"/>
+      <c r="M56" s="20">
+        <f t="shared" ref="M56:N56" si="4">SUM(M12:M15)</f>
+        <v>6837</v>
+      </c>
+      <c r="N56" s="20">
+        <f t="shared" si="4"/>
+        <v>1136</v>
+      </c>
+      <c r="O56" s="20">
+        <f t="shared" si="2"/>
         <v>7973</v>
       </c>
-      <c r="L56" s="20">
-        <f t="shared" si="0"/>
+      <c r="P56" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q56" s="20">
+        <f t="shared" ref="Q56" si="5">SUM(Q12:Q15)</f>
+        <v>13401</v>
+      </c>
+      <c r="R56" s="20">
+        <f t="shared" si="2"/>
         <v>624</v>
       </c>
-      <c r="M56" s="20">
-        <f t="shared" si="0"/>
+      <c r="S56" s="20">
+        <f t="shared" ref="S56" si="6">SUM(S12:S15)</f>
+        <v>17713</v>
+      </c>
+      <c r="T56" s="20">
+        <f t="shared" si="2"/>
         <v>7209</v>
       </c>
-      <c r="N56" s="20">
-        <f t="shared" si="0"/>
+      <c r="U56" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="V56" s="20">
+        <f t="shared" si="2"/>
         <v>4085</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W56" s="31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
         <v>161</v>
       </c>
@@ -4031,55 +5735,88 @@
         <v>1607</v>
       </c>
       <c r="C57" s="22">
-        <f t="shared" ref="C57:N57" si="1">SUM(C40:C44)</f>
+        <f t="shared" ref="C57:V57" si="7">SUM(C40:C44)</f>
         <v>50830</v>
       </c>
       <c r="D57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>1167</v>
       </c>
       <c r="E57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>14900</v>
       </c>
       <c r="F57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="G57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="H57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>551</v>
       </c>
       <c r="I57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J57" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J57:K57" si="8">SUM(J40:J44)</f>
+        <v>527</v>
+      </c>
+      <c r="K57" s="22">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="L57" s="22">
+        <f t="shared" si="7"/>
         <v>542</v>
       </c>
-      <c r="K57" s="22">
-        <f t="shared" si="1"/>
+      <c r="M57" s="22">
+        <f t="shared" ref="M57:N57" si="9">SUM(M40:M44)</f>
+        <v>23161</v>
+      </c>
+      <c r="N57" s="22">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O57" s="22">
+        <f t="shared" si="7"/>
         <v>23162</v>
       </c>
-      <c r="L57" s="22">
-        <f t="shared" si="1"/>
+      <c r="P57" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q57" s="22">
+        <f t="shared" ref="Q57" si="10">SUM(Q40:Q44)</f>
+        <v>23688</v>
+      </c>
+      <c r="R57" s="22">
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
-      <c r="M57" s="22">
-        <f t="shared" si="1"/>
+      <c r="S57" s="22">
+        <f t="shared" ref="S57" si="11">SUM(S40:S44)</f>
+        <v>23735</v>
+      </c>
+      <c r="T57" s="22">
+        <f t="shared" si="7"/>
         <v>2293</v>
       </c>
-      <c r="N57" s="22">
-        <f t="shared" si="1"/>
+      <c r="U57" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="V57" s="22">
+        <f t="shared" si="7"/>
         <v>856</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="W57" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
         <v>162</v>
       </c>
@@ -4088,63 +5825,94 @@
         <v>121111</v>
       </c>
       <c r="C58" s="21">
-        <f t="shared" ref="C58:N58" si="2">SUM(C2:C55)</f>
+        <f t="shared" ref="C58:V58" si="12">SUM(C2:C55)</f>
         <v>822492</v>
       </c>
       <c r="D58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>56872</v>
       </c>
       <c r="E58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>72899</v>
       </c>
       <c r="F58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>31797</v>
       </c>
       <c r="G58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>113205</v>
       </c>
       <c r="H58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>26327</v>
       </c>
       <c r="I58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>2394</v>
       </c>
       <c r="J58" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J58:K58" si="13">SUM(J2:J55)</f>
+        <v>318643</v>
+      </c>
+      <c r="K58" s="21">
+        <f t="shared" si="13"/>
+        <v>115837</v>
+      </c>
+      <c r="L58" s="21">
+        <f t="shared" si="12"/>
         <v>434480</v>
       </c>
-      <c r="K58" s="21">
-        <f t="shared" si="2"/>
+      <c r="M58" s="21">
+        <f t="shared" ref="M58:N58" si="14">SUM(M2:M55)</f>
+        <v>547927</v>
+      </c>
+      <c r="N58" s="21">
+        <f t="shared" si="14"/>
+        <v>49596</v>
+      </c>
+      <c r="O58" s="21">
+        <f t="shared" si="12"/>
         <v>597523</v>
       </c>
-      <c r="L58" s="21">
-        <f t="shared" si="2"/>
+      <c r="P58" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q58" s="21">
+        <f t="shared" ref="Q58" si="15">SUM(Q2:Q55)</f>
+        <v>866570</v>
+      </c>
+      <c r="R58" s="21">
+        <f t="shared" si="12"/>
         <v>28884</v>
       </c>
-      <c r="M58" s="21">
-        <f t="shared" si="2"/>
+      <c r="S58" s="21">
+        <f t="shared" ref="S58" si="16">SUM(S2:S55)</f>
+        <v>1060887</v>
+      </c>
+      <c r="T58" s="21">
+        <f t="shared" si="12"/>
         <v>162690</v>
       </c>
-      <c r="N58" s="21">
-        <f t="shared" si="2"/>
+      <c r="U58" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="V58" s="21">
+        <f t="shared" si="12"/>
         <v>151631</v>
       </c>
+      <c r="W58" s="33" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N58" xr:uid="{D90AFE98-8C78-4B1F-BEC8-FD4085F25E61}"/>
-  <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on circulation by item type spreadsheet for the year as run on January 1" sqref="L1" xr:uid="{78EE896E-66B5-4B14-8B20-F75A2CA9B99C}"/>
+  <autoFilter ref="A1:V58" xr:uid="{D90AFE98-8C78-4B1F-BEC8-FD4085F25E61}"/>
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on circulation by item type spreadsheet for the year as run on January 1" sqref="L1:S1" xr:uid="{78EE896E-66B5-4B14-8B20-F75A2CA9B99C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data from Item count by item type spreadsheet" sqref="C1" xr:uid="{C179746B-390C-44A4-AF6E-4A64D14353AD}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on the monthly circulation spreadsheet for the year as run on January 1" sqref="N1" xr:uid="{CD8BD2C4-A9FC-4A10-B4F4-EB4AEA221333}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on the monthly circulation spreadsheet for the year as run on January 1" sqref="B1 M1" xr:uid="{8891AF92-FA60-4235-8933-03E9BF764616}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on circulation by item type spreadsheet for the year as run on January 1" sqref="J1 K1" xr:uid="{706ABFFB-3D2A-4416-A3AE-F0A6BB32DC80}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data from Item count by item type spreadsheet for the year as run on January 1" sqref="I1 H1 G1 F1 E1 D1" xr:uid="{ADA05F97-168E-4E74-986A-EF2BBF782F8B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Based on the monthly circulation spreadsheet for the year as run on January 1" sqref="B1 T1:W1" xr:uid="{CD8BD2C4-A9FC-4A10-B4F4-EB4AEA221333}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Data from Item count by item type spreadsheet for the year as run on January 1" sqref="D1:K1" xr:uid="{ADA05F97-168E-4E74-986A-EF2BBF782F8B}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>